<commit_message>
Little change added to test cases
Change in 25th cases added
</commit_message>
<xml_diff>
--- a/gmail_signup_testCases.xlsx
+++ b/gmail_signup_testCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E8FD99-594E-473F-9B1F-FF158381903C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34296C66-B48E-4BBD-B326-1283371695B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,12 +415,6 @@
 4. Click on I agree button</t>
   </si>
   <si>
-    <t>1. Privacy and terms,more options,cancel and I agree button will be  present
-2. More options will open with radio button for different options
-3. Options for different settings can be selected
-4. Home page for Google account will open</t>
-  </si>
-  <si>
     <t>Chrome browser is open in windows pc</t>
   </si>
   <si>
@@ -550,6 +544,12 @@
   </si>
   <si>
     <t>Verify responsiveness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Privacy and terms,more options,cancel and I agree button will be  present
+2. More options will open with radio button for different options
+3. Options for different settings can be selected
+4. Home page for newly created Google account will open with welcome message </t>
   </si>
 </sst>
 </file>
@@ -1016,8 +1016,8 @@
   </sheetPr>
   <dimension ref="A1:AB929"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1089,7 @@
         <v>53</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>54</v>
@@ -1131,13 +1131,13 @@
         <v>56</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -1173,13 +1173,13 @@
         <v>57</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>58</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
@@ -1215,13 +1215,13 @@
         <v>48</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>59</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -1251,13 +1251,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>62</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>63</v>
@@ -1299,7 +1299,7 @@
         <v>50</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>60</v>
@@ -1341,13 +1341,13 @@
         <v>66</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>67</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
@@ -1383,13 +1383,13 @@
         <v>68</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -1428,10 +1428,10 @@
         <v>73</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
@@ -1515,7 +1515,7 @@
         <v>79</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
@@ -1554,10 +1554,10 @@
         <v>73</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
@@ -1590,16 +1590,16 @@
         <v>69</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
@@ -1635,7 +1635,7 @@
         <v>47</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>81</v>
@@ -1677,7 +1677,7 @@
         <v>83</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>84</v>
@@ -1806,7 +1806,7 @@
         <v>94</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>95</v>
@@ -2044,7 +2044,7 @@
       <c r="AA24" s="13"/>
       <c r="AB24" s="13"/>
     </row>
-    <row r="25" spans="1:28" s="14" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" s="14" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>111</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>115</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
@@ -2088,22 +2088,22 @@
     </row>
     <row r="26" spans="1:28" s="14" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="D26" s="24" t="s">
+      <c r="E26" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="F26" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>141</v>
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>

</xml_diff>